<commit_message>
Postcode and lecture location conversion
Postcode data download and manipulation. Building data conversion to CSV for Postgres import.
</commit_message>
<xml_diff>
--- a/data/lecture_locations/Buildings.xlsx
+++ b/data/lecture_locations/Buildings.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Year 3\Dissertation\Data Gathering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry\Documents\University\Year 3\Dissertation\UoP_Dissertation\data\lecture_locations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3383D2AD-22A4-42BA-AA8A-D58A02240208}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,7 +192,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -502,24 +503,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -539,7 +540,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -556,7 +557,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -573,7 +574,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -593,7 +594,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -607,7 +608,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -627,7 +628,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -641,7 +642,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -655,7 +656,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -669,7 +670,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -686,7 +687,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -703,7 +704,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -720,7 +721,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -737,7 +738,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -754,7 +755,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -768,7 +769,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -782,7 +783,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -799,7 +800,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -816,7 +817,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>

</xml_diff>